<commit_message>
add tree api document
</commit_message>
<xml_diff>
--- a/api-doc/tree.xlsx
+++ b/api-doc/tree.xlsx
@@ -1,26 +1,373 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="10560" yWindow="825" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="properties" sheetId="1" r:id="rId1"/>
+    <sheet name="events" sheetId="2" r:id="rId2"/>
+    <sheet name="methods" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="83">
+  <si>
+    <t>名字</t>
+  </si>
+  <si>
+    <t>类型</t>
+  </si>
+  <si>
+    <t>描述</t>
+  </si>
+  <si>
+    <t>默认</t>
+  </si>
+  <si>
+    <t>参数</t>
+  </si>
+  <si>
+    <t>url</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取服务端数据接口路径</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>object</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>给树配置本地数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expandCls</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树节点展开样式名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>collapseCls</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树节点收起样式名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>leafCls</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树叶子节点样式名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>folderCls</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树节点文件夹样式名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>folderOpenCls</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树节点文件夹打开样式名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>hasNodeIcon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>节点是否有图标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expandAll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树呈现是滞全部展开节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cache</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取远程数据是否本地缓存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>timeout</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>int</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取远程数据连接超时的时间（毫秒）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>queryParams</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取远程数据查询参数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onAjaxBeforeSend</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onAjaxComplete</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发送请求数据之前调用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请求数据完成后调用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onAjaxError</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>请求数据发生错误调用</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onClickNode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击节点事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e, node</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onClickRow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击节点行事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onExpanded</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>展开节点事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onCollapsed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收起节点事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>node</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onSelectedNode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>节点行被选中事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onExpandAll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>节点全部展开事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onCollapseAll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>节点全部收起事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onAfterRender</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>树渲染完成之后事件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>expandTo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectionNode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>selectionNodes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ids</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ecpandAll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>展开全部节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>collapseAll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收起全部节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择一批节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>checkAll</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>checked</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>prevNodeSelection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>isSelectionFolder</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以当前选中向上移位选中,参数决定是选中文件夹属性节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>nextNodeSelection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>以当前选中向下移位选中,参数决定是选中文件夹属性节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getSelectedNode</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取被选择的节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>getCheckedNodes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>获取被选中的节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clearAllSelection</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>清除所有选中节点</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选择指定树节点
+例如：
+$tbcontainer.tree('selectionNode', 5);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>展开指定树节点
+例如：
+$tbcontainer.tree('expandTo', 5);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>选中全部节点参数控制选中或未选中
+例如:
+$tbcontainer.tree('checkAll', true);</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -44,14 +391,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -341,13 +708,455 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+      <c r="D11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="2">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>